<commit_message>
add GS button with dialog refactor GUI by sections rename some bad names of functions
</commit_message>
<xml_diff>
--- a/resources/Летальность.xlsx
+++ b/resources/Летальность.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Лист1!$A$1:$AF$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Лист1!$A$1:$AF$5</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Лист1!$A$1:$AF$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Лист1!$A$1:$AF$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -419,7 +419,7 @@
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -787,7 +787,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:AF1"/>
+  <autoFilter ref="A1:AF5"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>